<commit_message>
Additional screenshot added in cucumber report
</commit_message>
<xml_diff>
--- a/testData/qa/Segmentation.xlsx
+++ b/testData/qa/Segmentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://operasolution-my.sharepoint.com/personal/naga_kumar_electrifai_com/Documents/newuiautomation/testData/qa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naga.kumar\customerAi\testData\qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="13_ncr:1_{1071E420-0D63-45A8-9B16-E6BA2C06E516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C28E03C4-E767-4713-B99D-FC56023B21E4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E33AA2-FFAB-4C0D-AA58-7060625585E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{EE76EA1F-E72F-46B2-BEA2-9E761BC260D6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{EE76EA1F-E72F-46B2-BEA2-9E761BC260D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Segmentation" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
   <si>
     <t>DataRowNum</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>segmentName</t>
+  </si>
+  <si>
+    <t>12_75</t>
   </si>
 </sst>
 </file>
@@ -533,19 +536,19 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="41.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.453125" customWidth="1"/>
+    <col min="4" max="4" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -586,7 +589,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -627,7 +630,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -686,19 +689,19 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -721,7 +724,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -755,17 +758,17 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -782,13 +785,16 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
       </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
       <c r="D2" t="s">
         <v>32</v>
       </c>
@@ -796,7 +802,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>

</xml_diff>